<commit_message>
[SonarQube] Fix more critical issues: duplicate literals, echo parentheses
- Fixed duplicate color literals (#3B82F6, #10B981, #EF4444) by defining constants
- Fixed echo parentheses in slopegraph/render.php
- Fixed duplicate '/blocks' literal in blocks.php register function
</commit_message>
<xml_diff>
--- a/sonarqube_issues_latest_month.xlsx
+++ b/sonarqube_issues_latest_month.xlsx
@@ -5931,7 +5931,7 @@
         </is>
       </c>
       <c r="F44" t="n">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="G44" t="inlineStr">
         <is>
@@ -5940,12 +5940,12 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>{'startLine': 315, 'endLine': 315, 'startOffset': 9, 'endOffset': 29}</t>
+          <t>{'startLine': 320, 'endLine': 320, 'startOffset': 9, 'endOffset': 29}</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/inc/blocks.php', 'textRange': {'startLine': 359, 'endLine': 359, 'startOffset': 4, 'endOffset': 10}, 'msg': '"return" statement.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/inc/blocks.php', 'textRange': {'startLine': 346, 'endLine': 346, 'startOffset': 12, 'endOffset': 18}, 'msg': '"return" statement.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/inc/blocks.php', 'textRange': {'startLine': 336, 'endLine': 336, 'startOffset': 8, 'endOffset': 14}, 'msg': '"return" statement.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/inc/blocks.php', 'textRange': {'startLine': 331, 'endLine': 331, 'startOffset': 8, 'endOffset': 14}, 'msg': '"return" statement.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/inc/blocks.php', 'textRange': {'startLine': 318, 'endLine': 318, 'startOffset': 8, 'endOffset': 14}, 'msg': '"return" statement.'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/inc/blocks.php', 'textRange': {'startLine': 364, 'endLine': 364, 'startOffset': 4, 'endOffset': 10}, 'msg': '"return" statement.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/inc/blocks.php', 'textRange': {'startLine': 351, 'endLine': 351, 'startOffset': 12, 'endOffset': 18}, 'msg': '"return" statement.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/inc/blocks.php', 'textRange': {'startLine': 341, 'endLine': 341, 'startOffset': 8, 'endOffset': 14}, 'msg': '"return" statement.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/inc/blocks.php', 'textRange': {'startLine': 336, 'endLine': 336, 'startOffset': 8, 'endOffset': 14}, 'msg': '"return" statement.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/inc/blocks.php', 'textRange': {'startLine': 323, 'endLine': 323, 'startOffset': 8, 'endOffset': 14}, 'msg': '"return" statement.'}]}]</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
@@ -19169,7 +19169,7 @@
         </is>
       </c>
       <c r="F148" t="n">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="G148" t="inlineStr">
         <is>
@@ -19178,7 +19178,7 @@
       </c>
       <c r="H148" t="inlineStr">
         <is>
-          <t>{'startLine': 275, 'endLine': 275, 'startOffset': 2, 'endOffset': 3}</t>
+          <t>{'startLine': 280, 'endLine': 280, 'startOffset': 2, 'endOffset': 3}</t>
         </is>
       </c>
       <c r="I148" t="inlineStr">
@@ -46887,9 +46887,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F360" t="n">
-        <v>5</v>
-      </c>
+      <c r="F360" t="inlineStr"/>
       <c r="G360" t="inlineStr">
         <is>
           <t>30bb9bc4febe39d6c1decf6380f28624</t>
@@ -46907,7 +46905,7 @@
       </c>
       <c r="J360" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K360" t="inlineStr">
@@ -46947,7 +46945,7 @@
       </c>
       <c r="R360" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T05:50:28+0000</t>
         </is>
       </c>
       <c r="S360" t="inlineStr">
@@ -46977,7 +46975,7 @@
       </c>
       <c r="X360" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y360" t="inlineStr">
@@ -46985,8 +46983,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z360" t="inlineStr"/>
-      <c r="AA360" t="inlineStr"/>
+      <c r="Z360" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA360" t="inlineStr">
+        <is>
+          <t>2025-12-28T05:50:28+0000</t>
+        </is>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -47390,17 +47396,17 @@
     <row r="364">
       <c r="A364" t="inlineStr">
         <is>
-          <t>AZthdkHsccKokRMjofv2</t>
+          <t>AZthdkHsccKokRMjofwD</t>
         </is>
       </c>
       <c r="B364" t="inlineStr">
         <is>
-          <t>Web:S6819</t>
+          <t>php:S121</t>
         </is>
       </c>
       <c r="C364" t="inlineStr">
         <is>
-          <t>MAJOR</t>
+          <t>CRITICAL</t>
         </is>
       </c>
       <c r="D364" t="inlineStr">
@@ -47413,17 +47419,15 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F364" t="n">
-        <v>41</v>
-      </c>
+      <c r="F364" t="inlineStr"/>
       <c r="G364" t="inlineStr">
         <is>
-          <t>837888434e0b076bb3523922bfa5d4cc</t>
+          <t>2a953bc8857b6b1aeee902cff023f159</t>
         </is>
       </c>
       <c r="H364" t="inlineStr">
         <is>
-          <t>{'startLine': 41, 'endLine': 43, 'startOffset': 0, 'endOffset': 67}</t>
+          <t>{'startLine': 41, 'endLine': 41, 'startOffset': 12, 'endOffset': 14}</t>
         </is>
       </c>
       <c r="I364" t="inlineStr">
@@ -47433,22 +47437,22 @@
       </c>
       <c r="J364" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K364" t="inlineStr">
         <is>
-          <t>Use &lt;img&gt; instead of the img role to ensure accessibility across all devices.</t>
+          <t>Add curly braces around the nested statement(s).</t>
         </is>
       </c>
       <c r="L364" t="inlineStr">
         <is>
-          <t>5min</t>
+          <t>2min</t>
         </is>
       </c>
       <c r="M364" t="inlineStr">
         <is>
-          <t>5min</t>
+          <t>2min</t>
         </is>
       </c>
       <c r="N364" t="inlineStr">
@@ -47463,7 +47467,7 @@
       </c>
       <c r="P364" t="inlineStr">
         <is>
-          <t>['accessibility']</t>
+          <t>['pitfall']</t>
         </is>
       </c>
       <c r="Q364" t="inlineStr">
@@ -47473,7 +47477,7 @@
       </c>
       <c r="R364" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T05:24:07+0000</t>
         </is>
       </c>
       <c r="S364" t="inlineStr">
@@ -47488,22 +47492,22 @@
       </c>
       <c r="U364" t="inlineStr">
         <is>
-          <t>CONVENTIONAL</t>
+          <t>CLEAR</t>
         </is>
       </c>
       <c r="V364" t="inlineStr">
         <is>
-          <t>CONSISTENT</t>
+          <t>INTENTIONAL</t>
         </is>
       </c>
       <c r="W364" t="inlineStr">
         <is>
-          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'MEDIUM'}]</t>
+          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'HIGH'}]</t>
         </is>
       </c>
       <c r="X364" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y364" t="inlineStr">
@@ -47511,13 +47515,21 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z364" t="inlineStr"/>
-      <c r="AA364" t="inlineStr"/>
+      <c r="Z364" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA364" t="inlineStr">
+        <is>
+          <t>2025-12-28T05:24:07+0000</t>
+        </is>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
         <is>
-          <t>AZthdkHsccKokRMjofwD</t>
+          <t>AZthdkHsccKokRMjofwE</t>
         </is>
       </c>
       <c r="B365" t="inlineStr">
@@ -47543,12 +47555,12 @@
       <c r="F365" t="inlineStr"/>
       <c r="G365" t="inlineStr">
         <is>
-          <t>2a953bc8857b6b1aeee902cff023f159</t>
+          <t>5aa8e0249fd6699e8cb0a395cb85e005</t>
         </is>
       </c>
       <c r="H365" t="inlineStr">
         <is>
-          <t>{'startLine': 41, 'endLine': 41, 'startOffset': 12, 'endOffset': 14}</t>
+          <t>{'startLine': 42, 'endLine': 42, 'startOffset': 12, 'endOffset': 14}</t>
         </is>
       </c>
       <c r="I365" t="inlineStr">
@@ -47650,17 +47662,17 @@
     <row r="366">
       <c r="A366" t="inlineStr">
         <is>
-          <t>AZthdkHsccKokRMjofwE</t>
+          <t>AZthdkHsccKokRMjofv2</t>
         </is>
       </c>
       <c r="B366" t="inlineStr">
         <is>
-          <t>php:S121</t>
+          <t>Web:S6819</t>
         </is>
       </c>
       <c r="C366" t="inlineStr">
         <is>
-          <t>CRITICAL</t>
+          <t>MAJOR</t>
         </is>
       </c>
       <c r="D366" t="inlineStr">
@@ -47673,15 +47685,17 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F366" t="inlineStr"/>
+      <c r="F366" t="n">
+        <v>43</v>
+      </c>
       <c r="G366" t="inlineStr">
         <is>
-          <t>5aa8e0249fd6699e8cb0a395cb85e005</t>
+          <t>837888434e0b076bb3523922bfa5d4cc</t>
         </is>
       </c>
       <c r="H366" t="inlineStr">
         <is>
-          <t>{'startLine': 42, 'endLine': 42, 'startOffset': 12, 'endOffset': 14}</t>
+          <t>{'startLine': 43, 'endLine': 45, 'startOffset': 0, 'endOffset': 67}</t>
         </is>
       </c>
       <c r="I366" t="inlineStr">
@@ -47691,22 +47705,22 @@
       </c>
       <c r="J366" t="inlineStr">
         <is>
-          <t>CLOSED</t>
+          <t>OPEN</t>
         </is>
       </c>
       <c r="K366" t="inlineStr">
         <is>
-          <t>Add curly braces around the nested statement(s).</t>
+          <t>Use &lt;img&gt; instead of the img role to ensure accessibility across all devices.</t>
         </is>
       </c>
       <c r="L366" t="inlineStr">
         <is>
-          <t>2min</t>
+          <t>5min</t>
         </is>
       </c>
       <c r="M366" t="inlineStr">
         <is>
-          <t>2min</t>
+          <t>5min</t>
         </is>
       </c>
       <c r="N366" t="inlineStr">
@@ -47721,7 +47735,7 @@
       </c>
       <c r="P366" t="inlineStr">
         <is>
-          <t>['pitfall']</t>
+          <t>['accessibility']</t>
         </is>
       </c>
       <c r="Q366" t="inlineStr">
@@ -47731,7 +47745,7 @@
       </c>
       <c r="R366" t="inlineStr">
         <is>
-          <t>2025-12-28T05:24:07+0000</t>
+          <t>2025-12-27T20:17:45+0000</t>
         </is>
       </c>
       <c r="S366" t="inlineStr">
@@ -47746,22 +47760,22 @@
       </c>
       <c r="U366" t="inlineStr">
         <is>
-          <t>CLEAR</t>
+          <t>CONVENTIONAL</t>
         </is>
       </c>
       <c r="V366" t="inlineStr">
         <is>
-          <t>INTENTIONAL</t>
+          <t>CONSISTENT</t>
         </is>
       </c>
       <c r="W366" t="inlineStr">
         <is>
-          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'HIGH'}]</t>
+          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'MEDIUM'}]</t>
         </is>
       </c>
       <c r="X366" t="inlineStr">
         <is>
-          <t>FIXED</t>
+          <t>OPEN</t>
         </is>
       </c>
       <c r="Y366" t="inlineStr">
@@ -47769,16 +47783,8 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z366" t="inlineStr">
-        <is>
-          <t>FIXED</t>
-        </is>
-      </c>
-      <c r="AA366" t="inlineStr">
-        <is>
-          <t>2025-12-28T05:24:07+0000</t>
-        </is>
-      </c>
+      <c r="Z366" t="inlineStr"/>
+      <c r="AA366" t="inlineStr"/>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -48870,9 +48876,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F375" t="n">
-        <v>5</v>
-      </c>
+      <c r="F375" t="inlineStr"/>
       <c r="G375" t="inlineStr">
         <is>
           <t>30bb9bc4febe39d6c1decf6380f28624</t>
@@ -48890,7 +48894,7 @@
       </c>
       <c r="J375" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K375" t="inlineStr">
@@ -48930,7 +48934,7 @@
       </c>
       <c r="R375" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T05:50:28+0000</t>
         </is>
       </c>
       <c r="S375" t="inlineStr">
@@ -48960,7 +48964,7 @@
       </c>
       <c r="X375" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y375" t="inlineStr">
@@ -48968,8 +48972,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z375" t="inlineStr"/>
-      <c r="AA375" t="inlineStr"/>
+      <c r="Z375" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA375" t="inlineStr">
+        <is>
+          <t>2025-12-28T05:50:28+0000</t>
+        </is>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -49373,17 +49385,17 @@
     <row r="379">
       <c r="A379" t="inlineStr">
         <is>
-          <t>AZthdkMJccKokRMjofyH</t>
+          <t>AZthdkMJccKokRMjofyI</t>
         </is>
       </c>
       <c r="B379" t="inlineStr">
         <is>
-          <t>Web:S6819</t>
+          <t>php:S1131</t>
         </is>
       </c>
       <c r="C379" t="inlineStr">
         <is>
-          <t>MAJOR</t>
+          <t>MINOR</t>
         </is>
       </c>
       <c r="D379" t="inlineStr">
@@ -49396,17 +49408,15 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F379" t="n">
-        <v>28</v>
-      </c>
+      <c r="F379" t="inlineStr"/>
       <c r="G379" t="inlineStr">
         <is>
-          <t>6dd333d664a2c33636695de04b74e674</t>
+          <t>5866d36f2fec02b3c321895b7fba113e</t>
         </is>
       </c>
       <c r="H379" t="inlineStr">
         <is>
-          <t>{'startLine': 28, 'endLine': 42, 'startOffset': 0, 'endOffset': 63}</t>
+          <t>{'startLine': 29, 'endLine': 29, 'startOffset': 23, 'endOffset': 24}</t>
         </is>
       </c>
       <c r="I379" t="inlineStr">
@@ -49416,22 +49426,22 @@
       </c>
       <c r="J379" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K379" t="inlineStr">
         <is>
-          <t>Use &lt;img&gt; instead of the img role to ensure accessibility across all devices.</t>
+          <t>Remove the useless trailing whitespaces at the end of this line.</t>
         </is>
       </c>
       <c r="L379" t="inlineStr">
         <is>
-          <t>5min</t>
+          <t>1min</t>
         </is>
       </c>
       <c r="M379" t="inlineStr">
         <is>
-          <t>5min</t>
+          <t>1min</t>
         </is>
       </c>
       <c r="N379" t="inlineStr">
@@ -49446,7 +49456,7 @@
       </c>
       <c r="P379" t="inlineStr">
         <is>
-          <t>['accessibility']</t>
+          <t>['convention', 'psr2']</t>
         </is>
       </c>
       <c r="Q379" t="inlineStr">
@@ -49456,7 +49466,7 @@
       </c>
       <c r="R379" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-27T22:13:31+0000</t>
         </is>
       </c>
       <c r="S379" t="inlineStr">
@@ -49471,7 +49481,7 @@
       </c>
       <c r="U379" t="inlineStr">
         <is>
-          <t>CONVENTIONAL</t>
+          <t>FORMATTED</t>
         </is>
       </c>
       <c r="V379" t="inlineStr">
@@ -49481,12 +49491,12 @@
       </c>
       <c r="W379" t="inlineStr">
         <is>
-          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'MEDIUM'}]</t>
+          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'LOW'}]</t>
         </is>
       </c>
       <c r="X379" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y379" t="inlineStr">
@@ -49494,23 +49504,31 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z379" t="inlineStr"/>
-      <c r="AA379" t="inlineStr"/>
+      <c r="Z379" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA379" t="inlineStr">
+        <is>
+          <t>2025-12-27T22:13:31+0000</t>
+        </is>
+      </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
         <is>
-          <t>AZthdkMJccKokRMjofyI</t>
+          <t>AZthdkMJccKokRMjofyH</t>
         </is>
       </c>
       <c r="B380" t="inlineStr">
         <is>
-          <t>php:S1131</t>
+          <t>Web:S6819</t>
         </is>
       </c>
       <c r="C380" t="inlineStr">
         <is>
-          <t>MINOR</t>
+          <t>MAJOR</t>
         </is>
       </c>
       <c r="D380" t="inlineStr">
@@ -49523,15 +49541,17 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F380" t="inlineStr"/>
+      <c r="F380" t="n">
+        <v>30</v>
+      </c>
       <c r="G380" t="inlineStr">
         <is>
-          <t>5866d36f2fec02b3c321895b7fba113e</t>
+          <t>6dd333d664a2c33636695de04b74e674</t>
         </is>
       </c>
       <c r="H380" t="inlineStr">
         <is>
-          <t>{'startLine': 29, 'endLine': 29, 'startOffset': 23, 'endOffset': 24}</t>
+          <t>{'startLine': 30, 'endLine': 44, 'startOffset': 0, 'endOffset': 63}</t>
         </is>
       </c>
       <c r="I380" t="inlineStr">
@@ -49541,22 +49561,22 @@
       </c>
       <c r="J380" t="inlineStr">
         <is>
-          <t>CLOSED</t>
+          <t>OPEN</t>
         </is>
       </c>
       <c r="K380" t="inlineStr">
         <is>
-          <t>Remove the useless trailing whitespaces at the end of this line.</t>
+          <t>Use &lt;img&gt; instead of the img role to ensure accessibility across all devices.</t>
         </is>
       </c>
       <c r="L380" t="inlineStr">
         <is>
-          <t>1min</t>
+          <t>5min</t>
         </is>
       </c>
       <c r="M380" t="inlineStr">
         <is>
-          <t>1min</t>
+          <t>5min</t>
         </is>
       </c>
       <c r="N380" t="inlineStr">
@@ -49571,7 +49591,7 @@
       </c>
       <c r="P380" t="inlineStr">
         <is>
-          <t>['convention', 'psr2']</t>
+          <t>['accessibility']</t>
         </is>
       </c>
       <c r="Q380" t="inlineStr">
@@ -49581,7 +49601,7 @@
       </c>
       <c r="R380" t="inlineStr">
         <is>
-          <t>2025-12-27T22:13:31+0000</t>
+          <t>2025-12-27T20:17:45+0000</t>
         </is>
       </c>
       <c r="S380" t="inlineStr">
@@ -49596,7 +49616,7 @@
       </c>
       <c r="U380" t="inlineStr">
         <is>
-          <t>FORMATTED</t>
+          <t>CONVENTIONAL</t>
         </is>
       </c>
       <c r="V380" t="inlineStr">
@@ -49606,12 +49626,12 @@
       </c>
       <c r="W380" t="inlineStr">
         <is>
-          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'LOW'}]</t>
+          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'MEDIUM'}]</t>
         </is>
       </c>
       <c r="X380" t="inlineStr">
         <is>
-          <t>FIXED</t>
+          <t>OPEN</t>
         </is>
       </c>
       <c r="Y380" t="inlineStr">
@@ -49619,16 +49639,8 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z380" t="inlineStr">
-        <is>
-          <t>FIXED</t>
-        </is>
-      </c>
-      <c r="AA380" t="inlineStr">
-        <is>
-          <t>2025-12-27T22:13:31+0000</t>
-        </is>
-      </c>
+      <c r="Z380" t="inlineStr"/>
+      <c r="AA380" t="inlineStr"/>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -50188,9 +50200,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F385" t="n">
-        <v>83</v>
-      </c>
+      <c r="F385" t="inlineStr"/>
       <c r="G385" t="inlineStr">
         <is>
           <t>fd3d87621e179265b32e0ad40ebeba28</t>
@@ -50198,17 +50208,17 @@
       </c>
       <c r="H385" t="inlineStr">
         <is>
-          <t>{'startLine': 83, 'endLine': 83, 'startOffset': 16, 'endOffset': 23}</t>
+          <t>{'startLine': 85, 'endLine': 85, 'startOffset': 16, 'endOffset': 23}</t>
         </is>
       </c>
       <c r="I385" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/flow-diagram/render.php', 'textRange': {'startLine': 84, 'endLine': 86, 'startOffset': 16, 'endOffset': 29}}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/flow-diagram/render.php', 'textRange': {'startLine': 86, 'endLine': 88, 'startOffset': 16, 'endOffset': 29}}]}]</t>
         </is>
       </c>
       <c r="J385" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K385" t="inlineStr">
@@ -50248,7 +50258,7 @@
       </c>
       <c r="R385" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T06:15:30+0000</t>
         </is>
       </c>
       <c r="S385" t="inlineStr">
@@ -50278,7 +50288,7 @@
       </c>
       <c r="X385" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y385" t="inlineStr">
@@ -50286,8 +50296,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z385" t="inlineStr"/>
-      <c r="AA385" t="inlineStr"/>
+      <c r="Z385" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA385" t="inlineStr">
+        <is>
+          <t>2025-12-28T06:15:30+0000</t>
+        </is>
+      </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
@@ -54124,9 +54142,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F415" t="n">
-        <v>5</v>
-      </c>
+      <c r="F415" t="inlineStr"/>
       <c r="G415" t="inlineStr">
         <is>
           <t>30bb9bc4febe39d6c1decf6380f28624</t>
@@ -54144,7 +54160,7 @@
       </c>
       <c r="J415" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K415" t="inlineStr">
@@ -54184,7 +54200,7 @@
       </c>
       <c r="R415" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T06:15:30+0000</t>
         </is>
       </c>
       <c r="S415" t="inlineStr">
@@ -54214,7 +54230,7 @@
       </c>
       <c r="X415" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y415" t="inlineStr">
@@ -54222,23 +54238,31 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z415" t="inlineStr"/>
-      <c r="AA415" t="inlineStr"/>
+      <c r="Z415" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA415" t="inlineStr">
+        <is>
+          <t>2025-12-28T06:15:30+0000</t>
+        </is>
+      </c>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
         <is>
-          <t>AZthdkLFccKokRMjofxs</t>
+          <t>AZthdkLFccKokRMjofxu</t>
         </is>
       </c>
       <c r="B416" t="inlineStr">
         <is>
-          <t>Web:S6819</t>
+          <t>php:S1131</t>
         </is>
       </c>
       <c r="C416" t="inlineStr">
         <is>
-          <t>MAJOR</t>
+          <t>MINOR</t>
         </is>
       </c>
       <c r="D416" t="inlineStr">
@@ -54251,9 +54275,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F416" t="n">
-        <v>27</v>
-      </c>
+      <c r="F416" t="inlineStr"/>
       <c r="G416" t="inlineStr">
         <is>
           <t>d11f9f21452bef005530c110ff1d0ad0</t>
@@ -54261,7 +54283,7 @@
       </c>
       <c r="H416" t="inlineStr">
         <is>
-          <t>{'startLine': 27, 'endLine': 41, 'startOffset': 0, 'endOffset': 83}</t>
+          <t>{'startLine': 27, 'endLine': 27, 'startOffset': 45, 'endOffset': 46}</t>
         </is>
       </c>
       <c r="I416" t="inlineStr">
@@ -54271,22 +54293,22 @@
       </c>
       <c r="J416" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K416" t="inlineStr">
         <is>
-          <t>Use &lt;img&gt; instead of the img role to ensure accessibility across all devices.</t>
+          <t>Remove the useless trailing whitespaces at the end of this line.</t>
         </is>
       </c>
       <c r="L416" t="inlineStr">
         <is>
-          <t>5min</t>
+          <t>1min</t>
         </is>
       </c>
       <c r="M416" t="inlineStr">
         <is>
-          <t>5min</t>
+          <t>1min</t>
         </is>
       </c>
       <c r="N416" t="inlineStr">
@@ -54301,7 +54323,7 @@
       </c>
       <c r="P416" t="inlineStr">
         <is>
-          <t>['accessibility']</t>
+          <t>['convention', 'psr2']</t>
         </is>
       </c>
       <c r="Q416" t="inlineStr">
@@ -54311,7 +54333,7 @@
       </c>
       <c r="R416" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-27T22:13:31+0000</t>
         </is>
       </c>
       <c r="S416" t="inlineStr">
@@ -54326,7 +54348,7 @@
       </c>
       <c r="U416" t="inlineStr">
         <is>
-          <t>CONVENTIONAL</t>
+          <t>FORMATTED</t>
         </is>
       </c>
       <c r="V416" t="inlineStr">
@@ -54336,12 +54358,12 @@
       </c>
       <c r="W416" t="inlineStr">
         <is>
-          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'MEDIUM'}]</t>
+          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'LOW'}]</t>
         </is>
       </c>
       <c r="X416" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y416" t="inlineStr">
@@ -54349,13 +54371,21 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z416" t="inlineStr"/>
-      <c r="AA416" t="inlineStr"/>
+      <c r="Z416" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA416" t="inlineStr">
+        <is>
+          <t>2025-12-27T22:13:31+0000</t>
+        </is>
+      </c>
     </row>
     <row r="417">
       <c r="A417" t="inlineStr">
         <is>
-          <t>AZthdkLFccKokRMjofxu</t>
+          <t>AZthdkLFccKokRMjofxv</t>
         </is>
       </c>
       <c r="B417" t="inlineStr">
@@ -54381,12 +54411,12 @@
       <c r="F417" t="inlineStr"/>
       <c r="G417" t="inlineStr">
         <is>
-          <t>d11f9f21452bef005530c110ff1d0ad0</t>
+          <t>55873bc3d3dc2b9a030b12ec5d49adbd</t>
         </is>
       </c>
       <c r="H417" t="inlineStr">
         <is>
-          <t>{'startLine': 27, 'endLine': 27, 'startOffset': 45, 'endOffset': 46}</t>
+          <t>{'startLine': 28, 'endLine': 28, 'startOffset': 18, 'endOffset': 19}</t>
         </is>
       </c>
       <c r="I417" t="inlineStr">
@@ -54488,17 +54518,17 @@
     <row r="418">
       <c r="A418" t="inlineStr">
         <is>
-          <t>AZthdkLFccKokRMjofxv</t>
+          <t>AZthdkLFccKokRMjofxs</t>
         </is>
       </c>
       <c r="B418" t="inlineStr">
         <is>
-          <t>php:S1131</t>
+          <t>Web:S6819</t>
         </is>
       </c>
       <c r="C418" t="inlineStr">
         <is>
-          <t>MINOR</t>
+          <t>MAJOR</t>
         </is>
       </c>
       <c r="D418" t="inlineStr">
@@ -54511,15 +54541,17 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F418" t="inlineStr"/>
+      <c r="F418" t="n">
+        <v>29</v>
+      </c>
       <c r="G418" t="inlineStr">
         <is>
-          <t>55873bc3d3dc2b9a030b12ec5d49adbd</t>
+          <t>d11f9f21452bef005530c110ff1d0ad0</t>
         </is>
       </c>
       <c r="H418" t="inlineStr">
         <is>
-          <t>{'startLine': 28, 'endLine': 28, 'startOffset': 18, 'endOffset': 19}</t>
+          <t>{'startLine': 29, 'endLine': 43, 'startOffset': 0, 'endOffset': 83}</t>
         </is>
       </c>
       <c r="I418" t="inlineStr">
@@ -54529,22 +54561,22 @@
       </c>
       <c r="J418" t="inlineStr">
         <is>
-          <t>CLOSED</t>
+          <t>OPEN</t>
         </is>
       </c>
       <c r="K418" t="inlineStr">
         <is>
-          <t>Remove the useless trailing whitespaces at the end of this line.</t>
+          <t>Use &lt;img&gt; instead of the img role to ensure accessibility across all devices.</t>
         </is>
       </c>
       <c r="L418" t="inlineStr">
         <is>
-          <t>1min</t>
+          <t>5min</t>
         </is>
       </c>
       <c r="M418" t="inlineStr">
         <is>
-          <t>1min</t>
+          <t>5min</t>
         </is>
       </c>
       <c r="N418" t="inlineStr">
@@ -54559,7 +54591,7 @@
       </c>
       <c r="P418" t="inlineStr">
         <is>
-          <t>['convention', 'psr2']</t>
+          <t>['accessibility']</t>
         </is>
       </c>
       <c r="Q418" t="inlineStr">
@@ -54569,7 +54601,7 @@
       </c>
       <c r="R418" t="inlineStr">
         <is>
-          <t>2025-12-27T22:13:31+0000</t>
+          <t>2025-12-27T20:17:45+0000</t>
         </is>
       </c>
       <c r="S418" t="inlineStr">
@@ -54584,7 +54616,7 @@
       </c>
       <c r="U418" t="inlineStr">
         <is>
-          <t>FORMATTED</t>
+          <t>CONVENTIONAL</t>
         </is>
       </c>
       <c r="V418" t="inlineStr">
@@ -54594,12 +54626,12 @@
       </c>
       <c r="W418" t="inlineStr">
         <is>
-          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'LOW'}]</t>
+          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'MEDIUM'}]</t>
         </is>
       </c>
       <c r="X418" t="inlineStr">
         <is>
-          <t>FIXED</t>
+          <t>OPEN</t>
         </is>
       </c>
       <c r="Y418" t="inlineStr">
@@ -54607,16 +54639,8 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z418" t="inlineStr">
-        <is>
-          <t>FIXED</t>
-        </is>
-      </c>
-      <c r="AA418" t="inlineStr">
-        <is>
-          <t>2025-12-27T22:13:31+0000</t>
-        </is>
-      </c>
+      <c r="Z418" t="inlineStr"/>
+      <c r="AA418" t="inlineStr"/>
     </row>
     <row r="419">
       <c r="A419" t="inlineStr">
@@ -54645,7 +54669,7 @@
         </is>
       </c>
       <c r="F419" t="n">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="G419" t="inlineStr">
         <is>
@@ -54654,7 +54678,7 @@
       </c>
       <c r="H419" t="inlineStr">
         <is>
-          <t>{'startLine': 70, 'endLine': 70, 'startOffset': 0, 'endOffset': 43}</t>
+          <t>{'startLine': 72, 'endLine': 72, 'startOffset': 0, 'endOffset': 43}</t>
         </is>
       </c>
       <c r="I419" t="inlineStr">
@@ -55037,9 +55061,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F422" t="n">
-        <v>84</v>
-      </c>
+      <c r="F422" t="inlineStr"/>
       <c r="G422" t="inlineStr">
         <is>
           <t>5d84531ac352f26cee414f5364354a7e</t>
@@ -55057,7 +55079,7 @@
       </c>
       <c r="J422" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K422" t="inlineStr">
@@ -55097,7 +55119,7 @@
       </c>
       <c r="R422" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T06:15:30+0000</t>
         </is>
       </c>
       <c r="S422" t="inlineStr">
@@ -55127,7 +55149,7 @@
       </c>
       <c r="X422" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y422" t="inlineStr">
@@ -55135,8 +55157,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z422" t="inlineStr"/>
-      <c r="AA422" t="inlineStr"/>
+      <c r="Z422" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA422" t="inlineStr">
+        <is>
+          <t>2025-12-28T06:15:30+0000</t>
+        </is>
+      </c>
     </row>
     <row r="423">
       <c r="A423" t="inlineStr">
@@ -55696,9 +55726,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F427" t="n">
-        <v>5</v>
-      </c>
+      <c r="F427" t="inlineStr"/>
       <c r="G427" t="inlineStr">
         <is>
           <t>30bb9bc4febe39d6c1decf6380f28624</t>
@@ -55716,7 +55744,7 @@
       </c>
       <c r="J427" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K427" t="inlineStr">
@@ -55756,7 +55784,7 @@
       </c>
       <c r="R427" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T06:15:30+0000</t>
         </is>
       </c>
       <c r="S427" t="inlineStr">
@@ -55786,7 +55814,7 @@
       </c>
       <c r="X427" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y427" t="inlineStr">
@@ -55794,8 +55822,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z427" t="inlineStr"/>
-      <c r="AA427" t="inlineStr"/>
+      <c r="Z427" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA427" t="inlineStr">
+        <is>
+          <t>2025-12-28T06:15:30+0000</t>
+        </is>
+      </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
@@ -56090,7 +56126,7 @@
         </is>
       </c>
       <c r="F430" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="G430" t="inlineStr">
         <is>
@@ -56099,7 +56135,7 @@
       </c>
       <c r="H430" t="inlineStr">
         <is>
-          <t>{'startLine': 24, 'endLine': 24, 'startOffset': 0, 'endOffset': 156}</t>
+          <t>{'startLine': 26, 'endLine': 26, 'startOffset': 0, 'endOffset': 156}</t>
         </is>
       </c>
       <c r="I430" t="inlineStr">
@@ -56350,7 +56386,7 @@
         </is>
       </c>
       <c r="F432" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G432" t="inlineStr">
         <is>
@@ -56359,12 +56395,12 @@
       </c>
       <c r="H432" t="inlineStr">
         <is>
-          <t>{'startLine': 51, 'endLine': 51, 'startOffset': 53, 'endOffset': 86}</t>
+          <t>{'startLine': 53, 'endLine': 53, 'startOffset': 53, 'endOffset': 86}</t>
         </is>
       </c>
       <c r="I432" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/slopegraph/render.php', 'textRange': {'startLine': 51, 'endLine': 51, 'startOffset': 38, 'endOffset': 39}, 'msg': 'Parent ternary operator'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/slopegraph/render.php', 'textRange': {'startLine': 53, 'endLine': 53, 'startOffset': 38, 'endOffset': 39}, 'msg': 'Parent ternary operator'}]}]</t>
         </is>
       </c>
       <c r="J432" t="inlineStr">
@@ -56477,7 +56513,7 @@
         </is>
       </c>
       <c r="F433" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="G433" t="inlineStr">
         <is>
@@ -56486,12 +56522,12 @@
       </c>
       <c r="H433" t="inlineStr">
         <is>
-          <t>{'startLine': 54, 'endLine': 54, 'startOffset': 91, 'endOffset': 128}</t>
+          <t>{'startLine': 56, 'endLine': 56, 'startOffset': 91, 'endOffset': 128}</t>
         </is>
       </c>
       <c r="I433" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/slopegraph/render.php', 'textRange': {'startLine': 54, 'endLine': 54, 'startOffset': 75, 'endOffset': 76}, 'msg': 'Parent ternary operator'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/slopegraph/render.php', 'textRange': {'startLine': 56, 'endLine': 56, 'startOffset': 75, 'endOffset': 76}, 'msg': 'Parent ternary operator'}]}]</t>
         </is>
       </c>
       <c r="J433" t="inlineStr">
@@ -56604,7 +56640,7 @@
         </is>
       </c>
       <c r="F434" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="G434" t="inlineStr">
         <is>
@@ -56613,12 +56649,12 @@
       </c>
       <c r="H434" t="inlineStr">
         <is>
-          <t>{'startLine': 56, 'endLine': 56, 'startOffset': 125, 'endOffset': 146}</t>
+          <t>{'startLine': 58, 'endLine': 58, 'startOffset': 125, 'endOffset': 146}</t>
         </is>
       </c>
       <c r="I434" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/slopegraph/render.php', 'textRange': {'startLine': 56, 'endLine': 56, 'startOffset': 116, 'endOffset': 117}, 'msg': 'Parent ternary operator'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/slopegraph/render.php', 'textRange': {'startLine': 58, 'endLine': 58, 'startOffset': 116, 'endOffset': 117}, 'msg': 'Parent ternary operator'}]}]</t>
         </is>
       </c>
       <c r="J434" t="inlineStr">
@@ -56731,7 +56767,7 @@
         </is>
       </c>
       <c r="F435" t="n">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G435" t="inlineStr">
         <is>
@@ -56740,12 +56776,12 @@
       </c>
       <c r="H435" t="inlineStr">
         <is>
-          <t>{'startLine': 58, 'endLine': 58, 'startOffset': 98, 'endOffset': 119}</t>
+          <t>{'startLine': 60, 'endLine': 60, 'startOffset': 98, 'endOffset': 119}</t>
         </is>
       </c>
       <c r="I435" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/slopegraph/render.php', 'textRange': {'startLine': 58, 'endLine': 58, 'startOffset': 89, 'endOffset': 90}, 'msg': 'Parent ternary operator'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/slopegraph/render.php', 'textRange': {'startLine': 60, 'endLine': 60, 'startOffset': 89, 'endOffset': 90}, 'msg': 'Parent ternary operator'}]}]</t>
         </is>
       </c>
       <c r="J435" t="inlineStr">
@@ -56834,17 +56870,17 @@
     <row r="436">
       <c r="A436" t="inlineStr">
         <is>
-          <t>AZthdkItccKokRMjofwY</t>
+          <t>AZthdkItccKokRMjofwQ</t>
         </is>
       </c>
       <c r="B436" t="inlineStr">
         <is>
-          <t>php:S3358</t>
+          <t>php:S1131</t>
         </is>
       </c>
       <c r="C436" t="inlineStr">
         <is>
-          <t>MAJOR</t>
+          <t>MINOR</t>
         </is>
       </c>
       <c r="D436" t="inlineStr">
@@ -56857,42 +56893,40 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F436" t="n">
-        <v>63</v>
-      </c>
+      <c r="F436" t="inlineStr"/>
       <c r="G436" t="inlineStr">
         <is>
-          <t>1552547d0dcb595dedba7268698d846f</t>
+          <t>43c3e3f65ea5e931d94d3caf2702f523</t>
         </is>
       </c>
       <c r="H436" t="inlineStr">
         <is>
-          <t>{'startLine': 63, 'endLine': 63, 'startOffset': 97, 'endOffset': 118}</t>
+          <t>{'startLine': 64, 'endLine': 64, 'startOffset': 153, 'endOffset': 154}</t>
         </is>
       </c>
       <c r="I436" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/slopegraph/render.php', 'textRange': {'startLine': 63, 'endLine': 63, 'startOffset': 89, 'endOffset': 90}, 'msg': 'Parent ternary operator'}]}]</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="J436" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K436" t="inlineStr">
         <is>
-          <t>Extract this nested ternary operation into an independent statement.</t>
+          <t>Remove the useless trailing whitespaces at the end of this line.</t>
         </is>
       </c>
       <c r="L436" t="inlineStr">
         <is>
-          <t>5min</t>
+          <t>1min</t>
         </is>
       </c>
       <c r="M436" t="inlineStr">
         <is>
-          <t>5min</t>
+          <t>1min</t>
         </is>
       </c>
       <c r="N436" t="inlineStr">
@@ -56907,7 +56941,7 @@
       </c>
       <c r="P436" t="inlineStr">
         <is>
-          <t>['confusing']</t>
+          <t>['convention', 'psr2']</t>
         </is>
       </c>
       <c r="Q436" t="inlineStr">
@@ -56917,7 +56951,7 @@
       </c>
       <c r="R436" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-27T22:13:31+0000</t>
         </is>
       </c>
       <c r="S436" t="inlineStr">
@@ -56932,22 +56966,22 @@
       </c>
       <c r="U436" t="inlineStr">
         <is>
-          <t>CLEAR</t>
+          <t>FORMATTED</t>
         </is>
       </c>
       <c r="V436" t="inlineStr">
         <is>
-          <t>INTENTIONAL</t>
+          <t>CONSISTENT</t>
         </is>
       </c>
       <c r="W436" t="inlineStr">
         <is>
-          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'MEDIUM'}]</t>
+          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'LOW'}]</t>
         </is>
       </c>
       <c r="X436" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y436" t="inlineStr">
@@ -56955,23 +56989,31 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z436" t="inlineStr"/>
-      <c r="AA436" t="inlineStr"/>
+      <c r="Z436" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA436" t="inlineStr">
+        <is>
+          <t>2025-12-27T22:13:31+0000</t>
+        </is>
+      </c>
     </row>
     <row r="437">
       <c r="A437" t="inlineStr">
         <is>
-          <t>AZthdkItccKokRMjofwQ</t>
+          <t>AZthdkItccKokRMjofwY</t>
         </is>
       </c>
       <c r="B437" t="inlineStr">
         <is>
-          <t>php:S1131</t>
+          <t>php:S3358</t>
         </is>
       </c>
       <c r="C437" t="inlineStr">
         <is>
-          <t>MINOR</t>
+          <t>MAJOR</t>
         </is>
       </c>
       <c r="D437" t="inlineStr">
@@ -56984,40 +57026,42 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F437" t="inlineStr"/>
+      <c r="F437" t="n">
+        <v>65</v>
+      </c>
       <c r="G437" t="inlineStr">
         <is>
-          <t>43c3e3f65ea5e931d94d3caf2702f523</t>
+          <t>1552547d0dcb595dedba7268698d846f</t>
         </is>
       </c>
       <c r="H437" t="inlineStr">
         <is>
-          <t>{'startLine': 64, 'endLine': 64, 'startOffset': 153, 'endOffset': 154}</t>
+          <t>{'startLine': 65, 'endLine': 65, 'startOffset': 97, 'endOffset': 118}</t>
         </is>
       </c>
       <c r="I437" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/slopegraph/render.php', 'textRange': {'startLine': 65, 'endLine': 65, 'startOffset': 89, 'endOffset': 90}, 'msg': 'Parent ternary operator'}]}]</t>
         </is>
       </c>
       <c r="J437" t="inlineStr">
         <is>
-          <t>CLOSED</t>
+          <t>OPEN</t>
         </is>
       </c>
       <c r="K437" t="inlineStr">
         <is>
-          <t>Remove the useless trailing whitespaces at the end of this line.</t>
+          <t>Extract this nested ternary operation into an independent statement.</t>
         </is>
       </c>
       <c r="L437" t="inlineStr">
         <is>
-          <t>1min</t>
+          <t>5min</t>
         </is>
       </c>
       <c r="M437" t="inlineStr">
         <is>
-          <t>1min</t>
+          <t>5min</t>
         </is>
       </c>
       <c r="N437" t="inlineStr">
@@ -57032,7 +57076,7 @@
       </c>
       <c r="P437" t="inlineStr">
         <is>
-          <t>['convention', 'psr2']</t>
+          <t>['confusing']</t>
         </is>
       </c>
       <c r="Q437" t="inlineStr">
@@ -57042,7 +57086,7 @@
       </c>
       <c r="R437" t="inlineStr">
         <is>
-          <t>2025-12-27T22:13:31+0000</t>
+          <t>2025-12-27T20:17:45+0000</t>
         </is>
       </c>
       <c r="S437" t="inlineStr">
@@ -57057,22 +57101,22 @@
       </c>
       <c r="U437" t="inlineStr">
         <is>
-          <t>FORMATTED</t>
+          <t>CLEAR</t>
         </is>
       </c>
       <c r="V437" t="inlineStr">
         <is>
-          <t>CONSISTENT</t>
+          <t>INTENTIONAL</t>
         </is>
       </c>
       <c r="W437" t="inlineStr">
         <is>
-          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'LOW'}]</t>
+          <t>[{'softwareQuality': 'MAINTAINABILITY', 'severity': 'MEDIUM'}]</t>
         </is>
       </c>
       <c r="X437" t="inlineStr">
         <is>
-          <t>FIXED</t>
+          <t>OPEN</t>
         </is>
       </c>
       <c r="Y437" t="inlineStr">
@@ -57080,16 +57124,8 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z437" t="inlineStr">
-        <is>
-          <t>FIXED</t>
-        </is>
-      </c>
-      <c r="AA437" t="inlineStr">
-        <is>
-          <t>2025-12-27T22:13:31+0000</t>
-        </is>
-      </c>
+      <c r="Z437" t="inlineStr"/>
+      <c r="AA437" t="inlineStr"/>
     </row>
     <row r="438">
       <c r="A438" t="inlineStr">
@@ -57118,7 +57154,7 @@
         </is>
       </c>
       <c r="F438" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="G438" t="inlineStr">
         <is>
@@ -57127,12 +57163,12 @@
       </c>
       <c r="H438" t="inlineStr">
         <is>
-          <t>{'startLine': 64, 'endLine': 64, 'startOffset': 97, 'endOffset': 118}</t>
+          <t>{'startLine': 66, 'endLine': 66, 'startOffset': 97, 'endOffset': 118}</t>
         </is>
       </c>
       <c r="I438" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/slopegraph/render.php', 'textRange': {'startLine': 64, 'endLine': 64, 'startOffset': 89, 'endOffset': 90}, 'msg': 'Parent ternary operator'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/slopegraph/render.php', 'textRange': {'startLine': 66, 'endLine': 66, 'startOffset': 89, 'endOffset': 90}, 'msg': 'Parent ternary operator'}]}]</t>
         </is>
       </c>
       <c r="J438" t="inlineStr">
@@ -57245,7 +57281,7 @@
         </is>
       </c>
       <c r="F439" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G439" t="inlineStr">
         <is>
@@ -57254,7 +57290,7 @@
       </c>
       <c r="H439" t="inlineStr">
         <is>
-          <t>{'startLine': 68, 'endLine': 68, 'startOffset': 31, 'endOffset': 61}</t>
+          <t>{'startLine': 70, 'endLine': 70, 'startOffset': 31, 'endOffset': 61}</t>
         </is>
       </c>
       <c r="I439" t="inlineStr">
@@ -58018,9 +58054,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F445" t="n">
-        <v>5</v>
-      </c>
+      <c r="F445" t="inlineStr"/>
       <c r="G445" t="inlineStr">
         <is>
           <t>30bb9bc4febe39d6c1decf6380f28624</t>
@@ -58038,7 +58072,7 @@
       </c>
       <c r="J445" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K445" t="inlineStr">
@@ -58078,7 +58112,7 @@
       </c>
       <c r="R445" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T06:15:30+0000</t>
         </is>
       </c>
       <c r="S445" t="inlineStr">
@@ -58108,7 +58142,7 @@
       </c>
       <c r="X445" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y445" t="inlineStr">
@@ -58116,8 +58150,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z445" t="inlineStr"/>
-      <c r="AA445" t="inlineStr"/>
+      <c r="Z445" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA445" t="inlineStr">
+        <is>
+          <t>2025-12-28T06:15:30+0000</t>
+        </is>
+      </c>
     </row>
     <row r="446">
       <c r="A446" t="inlineStr">
@@ -58811,7 +58853,7 @@
         </is>
       </c>
       <c r="F451" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="G451" t="inlineStr">
         <is>
@@ -58820,7 +58862,7 @@
       </c>
       <c r="H451" t="inlineStr">
         <is>
-          <t>{'startLine': 50, 'endLine': 51, 'startOffset': 0, 'endOffset': 78}</t>
+          <t>{'startLine': 52, 'endLine': 53, 'startOffset': 0, 'endOffset': 78}</t>
         </is>
       </c>
       <c r="I451" t="inlineStr">
@@ -61586,7 +61628,7 @@
         </is>
       </c>
       <c r="F472" t="n">
-        <v>231</v>
+        <v>236</v>
       </c>
       <c r="G472" t="inlineStr">
         <is>
@@ -61595,7 +61637,7 @@
       </c>
       <c r="H472" t="inlineStr">
         <is>
-          <t>{'startLine': 231, 'endLine': 231, 'startOffset': 35, 'endOffset': 44}</t>
+          <t>{'startLine': 236, 'endLine': 236, 'startOffset': 35, 'endOffset': 44}</t>
         </is>
       </c>
       <c r="I472" t="inlineStr">
@@ -61846,7 +61888,7 @@
         </is>
       </c>
       <c r="F474" t="n">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="G474" t="inlineStr">
         <is>
@@ -61855,7 +61897,7 @@
       </c>
       <c r="H474" t="inlineStr">
         <is>
-          <t>{'startLine': 288, 'endLine': 288, 'startOffset': 35, 'endOffset': 44}</t>
+          <t>{'startLine': 293, 'endLine': 293, 'startOffset': 35, 'endOffset': 44}</t>
         </is>
       </c>
       <c r="I474" t="inlineStr">
@@ -61973,7 +62015,7 @@
         </is>
       </c>
       <c r="F475" t="n">
-        <v>315</v>
+        <v>320</v>
       </c>
       <c r="G475" t="inlineStr">
         <is>
@@ -61982,7 +62024,7 @@
       </c>
       <c r="H475" t="inlineStr">
         <is>
-          <t>{'startLine': 315, 'endLine': 315, 'startOffset': 9, 'endOffset': 29}</t>
+          <t>{'startLine': 320, 'endLine': 320, 'startOffset': 9, 'endOffset': 29}</t>
         </is>
       </c>
       <c r="I475" t="inlineStr">
@@ -64446,7 +64488,7 @@
         </is>
       </c>
       <c r="F494" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G494" t="inlineStr">
         <is>
@@ -64455,12 +64497,12 @@
       </c>
       <c r="H494" t="inlineStr">
         <is>
-          <t>{'startLine': 101, 'endLine': 101, 'startOffset': 140, 'endOffset': 150}</t>
+          <t>{'startLine': 103, 'endLine': 103, 'startOffset': 140, 'endOffset': 150}</t>
         </is>
       </c>
       <c r="I494" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 135, 'endLine': 135, 'startOffset': 122, 'endOffset': 132}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 181, 'endLine': 181, 'startOffset': 131, 'endOffset': 141}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 206, 'endLine': 206, 'startOffset': 141, 'endOffset': 151}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 237, 'endLine': 237, 'startOffset': 140, 'endOffset': 150}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 263, 'endLine': 263, 'startOffset': 126, 'endOffset': 136}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 327, 'endLine': 327, 'startOffset': 80, 'endOffset': 90}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 506, 'endLine': 506, 'startOffset': 123, 'endOffset': 133}, 'msg': 'Duplication.'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 137, 'endLine': 137, 'startOffset': 122, 'endOffset': 132}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 187, 'endLine': 187, 'startOffset': 131, 'endOffset': 141}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 212, 'endLine': 212, 'startOffset': 141, 'endOffset': 151}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 243, 'endLine': 243, 'startOffset': 140, 'endOffset': 150}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 269, 'endLine': 269, 'startOffset': 126, 'endOffset': 136}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 337, 'endLine': 337, 'startOffset': 80, 'endOffset': 90}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 516, 'endLine': 516, 'startOffset': 123, 'endOffset': 133}, 'msg': 'Duplication.'}]}]</t>
         </is>
       </c>
       <c r="J494" t="inlineStr">
@@ -64705,9 +64747,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F496" t="n">
-        <v>34</v>
-      </c>
+      <c r="F496" t="inlineStr"/>
       <c r="G496" t="inlineStr">
         <is>
           <t>c471a0e582b92bcebf7e32e806f72030</t>
@@ -64725,7 +64765,7 @@
       </c>
       <c r="J496" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K496" t="inlineStr">
@@ -64765,7 +64805,7 @@
       </c>
       <c r="R496" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T05:57:21+0000</t>
         </is>
       </c>
       <c r="S496" t="inlineStr">
@@ -64795,7 +64835,7 @@
       </c>
       <c r="X496" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y496" t="inlineStr">
@@ -64803,8 +64843,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z496" t="inlineStr"/>
-      <c r="AA496" t="inlineStr"/>
+      <c r="Z496" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA496" t="inlineStr">
+        <is>
+          <t>2025-12-28T05:57:21+0000</t>
+        </is>
+      </c>
     </row>
     <row r="497">
       <c r="A497" t="inlineStr">
@@ -64833,7 +64881,7 @@
         </is>
       </c>
       <c r="F497" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="G497" t="inlineStr">
         <is>
@@ -64842,12 +64890,12 @@
       </c>
       <c r="H497" t="inlineStr">
         <is>
-          <t>{'startLine': 45, 'endLine': 45, 'startOffset': 65, 'endOffset': 74}</t>
+          <t>{'startLine': 47, 'endLine': 47, 'startOffset': 65, 'endOffset': 74}</t>
         </is>
       </c>
       <c r="I497" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 46, 'endLine': 46, 'startOffset': 31, 'endOffset': 40}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 50, 'endLine': 50, 'startOffset': 56, 'endOffset': 65}, 'msg': 'Duplication.'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 48, 'endLine': 48, 'startOffset': 31, 'endOffset': 40}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 52, 'endLine': 52, 'startOffset': 56, 'endOffset': 65}, 'msg': 'Duplication.'}]}]</t>
         </is>
       </c>
       <c r="J497" t="inlineStr">
@@ -64960,7 +65008,7 @@
         </is>
       </c>
       <c r="F498" t="n">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="G498" t="inlineStr">
         <is>
@@ -64969,12 +65017,12 @@
       </c>
       <c r="H498" t="inlineStr">
         <is>
-          <t>{'startLine': 48, 'endLine': 48, 'startOffset': 32, 'endOffset': 41}</t>
+          <t>{'startLine': 50, 'endLine': 50, 'startOffset': 32, 'endOffset': 41}</t>
         </is>
       </c>
       <c r="I498" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 50, 'endLine': 50, 'startOffset': 45, 'endOffset': 54}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 56, 'endLine': 56, 'startOffset': 18, 'endOffset': 27}, 'msg': 'Duplication.'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 52, 'endLine': 52, 'startOffset': 45, 'endOffset': 54}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 58, 'endLine': 58, 'startOffset': 18, 'endOffset': 27}, 'msg': 'Duplication.'}]}]</t>
         </is>
       </c>
       <c r="J498" t="inlineStr">
@@ -65087,7 +65135,7 @@
         </is>
       </c>
       <c r="F499" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G499" t="inlineStr">
         <is>
@@ -65096,12 +65144,12 @@
       </c>
       <c r="H499" t="inlineStr">
         <is>
-          <t>{'startLine': 92, 'endLine': 92, 'startOffset': 81, 'endOffset': 89}</t>
+          <t>{'startLine': 94, 'endLine': 94, 'startOffset': 81, 'endOffset': 89}</t>
         </is>
       </c>
       <c r="I499" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 122, 'endLine': 122, 'startOffset': 82, 'endOffset': 90}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 127, 'endLine': 127, 'startOffset': 105, 'endOffset': 113}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 195, 'endLine': 195, 'startOffset': 109, 'endOffset': 117}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 251, 'endLine': 251, 'startOffset': 109, 'endOffset': 117}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 305, 'endLine': 305, 'startOffset': 78, 'endOffset': 86}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 310, 'endLine': 310, 'startOffset': 101, 'endOffset': 109}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 360, 'endLine': 360, 'startOffset': 72, 'endOffset': 80}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 482, 'endLine': 482, 'startOffset': 101, 'endOffset': 109}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 485, 'endLine': 485, 'startOffset': 75, 'endOffset': 83}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 512, 'endLine': 512, 'startOffset': 88, 'endOffset': 96}, 'msg': 'Duplication.'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 124, 'endLine': 124, 'startOffset': 82, 'endOffset': 90}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 129, 'endLine': 129, 'startOffset': 105, 'endOffset': 113}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 201, 'endLine': 201, 'startOffset': 109, 'endOffset': 117}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 257, 'endLine': 257, 'startOffset': 109, 'endOffset': 117}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 315, 'endLine': 315, 'startOffset': 78, 'endOffset': 86}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 320, 'endLine': 320, 'startOffset': 101, 'endOffset': 109}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 370, 'endLine': 370, 'startOffset': 72, 'endOffset': 80}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 492, 'endLine': 492, 'startOffset': 101, 'endOffset': 109}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 495, 'endLine': 495, 'startOffset': 75, 'endOffset': 83}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 522, 'endLine': 522, 'startOffset': 88, 'endOffset': 96}, 'msg': 'Duplication.'}]}]</t>
         </is>
       </c>
       <c r="J499" t="inlineStr">
@@ -65214,7 +65262,7 @@
         </is>
       </c>
       <c r="F500" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G500" t="inlineStr">
         <is>
@@ -65223,12 +65271,12 @@
       </c>
       <c r="H500" t="inlineStr">
         <is>
-          <t>{'startLine': 92, 'endLine': 92, 'startOffset': 53, 'endOffset': 61}</t>
+          <t>{'startLine': 94, 'endLine': 94, 'startOffset': 53, 'endOffset': 61}</t>
         </is>
       </c>
       <c r="I500" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 122, 'endLine': 122, 'startOffset': 66, 'endOffset': 74}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 127, 'endLine': 127, 'startOffset': 58, 'endOffset': 66}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 195, 'endLine': 195, 'startOffset': 62, 'endOffset': 70}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 251, 'endLine': 251, 'startOffset': 62, 'endOffset': 70}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 305, 'endLine': 305, 'startOffset': 62, 'endOffset': 70}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 310, 'endLine': 310, 'startOffset': 54, 'endOffset': 62}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 360, 'endLine': 360, 'startOffset': 49, 'endOffset': 57}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 482, 'endLine': 482, 'startOffset': 54, 'endOffset': 62}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 485, 'endLine': 485, 'startOffset': 54, 'endOffset': 62}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 512, 'endLine': 512, 'startOffset': 64, 'endOffset': 72}, 'msg': 'Duplication.'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 124, 'endLine': 124, 'startOffset': 66, 'endOffset': 74}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 129, 'endLine': 129, 'startOffset': 58, 'endOffset': 66}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 201, 'endLine': 201, 'startOffset': 62, 'endOffset': 70}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 257, 'endLine': 257, 'startOffset': 62, 'endOffset': 70}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 315, 'endLine': 315, 'startOffset': 62, 'endOffset': 70}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 320, 'endLine': 320, 'startOffset': 54, 'endOffset': 62}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 370, 'endLine': 370, 'startOffset': 49, 'endOffset': 57}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 492, 'endLine': 492, 'startOffset': 54, 'endOffset': 62}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 495, 'endLine': 495, 'startOffset': 54, 'endOffset': 62}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 522, 'endLine': 522, 'startOffset': 64, 'endOffset': 72}, 'msg': 'Duplication.'}]}]</t>
         </is>
       </c>
       <c r="J500" t="inlineStr">
@@ -65341,7 +65389,7 @@
         </is>
       </c>
       <c r="F501" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G501" t="inlineStr">
         <is>
@@ -65350,12 +65398,12 @@
       </c>
       <c r="H501" t="inlineStr">
         <is>
-          <t>{'startLine': 92, 'endLine': 92, 'startOffset': 97, 'endOffset': 105}</t>
+          <t>{'startLine': 94, 'endLine': 94, 'startOffset': 97, 'endOffset': 105}</t>
         </is>
       </c>
       <c r="I501" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 122, 'endLine': 122, 'startOffset': 127, 'endOffset': 135}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 127, 'endLine': 127, 'startOffset': 150, 'endOffset': 158}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 195, 'endLine': 195, 'startOffset': 154, 'endOffset': 162}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 251, 'endLine': 251, 'startOffset': 154, 'endOffset': 162}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 305, 'endLine': 305, 'startOffset': 123, 'endOffset': 131}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 310, 'endLine': 310, 'startOffset': 146, 'endOffset': 154}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 360, 'endLine': 360, 'startOffset': 95, 'endOffset': 103}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 482, 'endLine': 482, 'startOffset': 146, 'endOffset': 154}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 485, 'endLine': 485, 'startOffset': 120, 'endOffset': 128}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 512, 'endLine': 512, 'startOffset': 109, 'endOffset': 117}, 'msg': 'Duplication.'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 124, 'endLine': 124, 'startOffset': 127, 'endOffset': 135}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 129, 'endLine': 129, 'startOffset': 150, 'endOffset': 158}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 201, 'endLine': 201, 'startOffset': 154, 'endOffset': 162}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 257, 'endLine': 257, 'startOffset': 154, 'endOffset': 162}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 315, 'endLine': 315, 'startOffset': 123, 'endOffset': 131}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 320, 'endLine': 320, 'startOffset': 146, 'endOffset': 154}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 370, 'endLine': 370, 'startOffset': 95, 'endOffset': 103}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 492, 'endLine': 492, 'startOffset': 146, 'endOffset': 154}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 495, 'endLine': 495, 'startOffset': 120, 'endOffset': 128}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 522, 'endLine': 522, 'startOffset': 109, 'endOffset': 117}, 'msg': 'Duplication.'}]}]</t>
         </is>
       </c>
       <c r="J501" t="inlineStr">
@@ -65468,7 +65516,7 @@
         </is>
       </c>
       <c r="F502" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G502" t="inlineStr">
         <is>
@@ -65477,12 +65525,12 @@
       </c>
       <c r="H502" t="inlineStr">
         <is>
-          <t>{'startLine': 101, 'endLine': 101, 'startOffset': 61, 'endOffset': 68}</t>
+          <t>{'startLine': 103, 'endLine': 103, 'startOffset': 61, 'endOffset': 68}</t>
         </is>
       </c>
       <c r="I502" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 104, 'endLine': 104, 'startOffset': 67, 'endOffset': 74}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 108, 'endLine': 108, 'startOffset': 84, 'endOffset': 91}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 135, 'endLine': 135, 'startOffset': 48, 'endOffset': 55}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 139, 'endLine': 139, 'startOffset': 71, 'endOffset': 78}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 143, 'endLine': 143, 'startOffset': 67, 'endOffset': 74}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 181, 'endLine': 181, 'startOffset': 64, 'endOffset': 71}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 185, 'endLine': 185, 'startOffset': 71, 'endOffset': 78}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 206, 'endLine': 206, 'startOffset': 56, 'endOffset': 63}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 210, 'endLine': 210, 'startOffset': 71, 'endOffset': 78}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 237, 'endLine': 237, 'startOffset': 69, 'endOffset': 76}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 240, 'endLine': 240, 'startOffset': 71, 'endOffset': 78}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 263, 'endLine': 263, 'startOffset': 56, 'endOffset': 63}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 266, 'endLine': 266, 'startOffset': 79, 'endOffset': 86}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 279, 'endLine': 279, 'startOffset': 48, 'endOffset': 55}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 280, 'endLine': 280, 'startOffset': 55, 'endOffset': 62}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 342, 'endLine': 342, 'startOffset': 52, 'endOffset': 59}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 350, 'endLine': 350, 'startOffset': 44, 'endOffset': 51}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 361, 'endLine': 361, 'startOffset': 55, 'endOffset': 62}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 405, 'endLine': 405, 'startOffset': 54, 'endOffset': 61}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 413, 'endLine': 413, 'startOffset': 51, 'endOffset': 58}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 414, 'endLine': 414, 'startOffset': 51, 'endOffset': 58}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 423, 'endLine': 423, 'startOffset': 55, 'endOffset': 62}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 424, 'endLine': 424, 'startOffset': 62, 'endOffset': 69}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 506, 'endLine': 506, 'startOffset': 44, 'endOffset': 51}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 519, 'endLine': 519, 'startOffset': 67, 'endOffset': 74}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 532, 'endLine': 532, 'startOffset': 63, 'endOffset': 70}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 538, 'endLine': 538, 'startOffset': 57, 'endOffset': 64}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 539, 'endLine': 539, 'startOffset': 64, 'endOffset': 71}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 540, 'endLine': 540, 'startOffset': 64, 'endOffset': 71}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 541, 'endLine': 541, 'startOffset': 64, 'endOffset': 71}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 542, 'endLine': 542, 'startOffset': 65, 'endOffset': 72}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 543, 'endLine': 543, 'startOffset': 65, 'endOffset': 72}, 'msg': 'Duplication.'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 106, 'endLine': 106, 'startOffset': 67, 'endOffset': 74}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 110, 'endLine': 110, 'startOffset': 84, 'endOffset': 91}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 137, 'endLine': 137, 'startOffset': 48, 'endOffset': 55}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 141, 'endLine': 141, 'startOffset': 71, 'endOffset': 78}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 145, 'endLine': 145, 'startOffset': 67, 'endOffset': 74}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 187, 'endLine': 187, 'startOffset': 64, 'endOffset': 71}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 191, 'endLine': 191, 'startOffset': 71, 'endOffset': 78}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 212, 'endLine': 212, 'startOffset': 56, 'endOffset': 63}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 216, 'endLine': 216, 'startOffset': 71, 'endOffset': 78}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 243, 'endLine': 243, 'startOffset': 69, 'endOffset': 76}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 246, 'endLine': 246, 'startOffset': 71, 'endOffset': 78}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 269, 'endLine': 269, 'startOffset': 56, 'endOffset': 63}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 272, 'endLine': 272, 'startOffset': 79, 'endOffset': 86}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 285, 'endLine': 285, 'startOffset': 48, 'endOffset': 55}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 286, 'endLine': 286, 'startOffset': 55, 'endOffset': 62}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 352, 'endLine': 352, 'startOffset': 52, 'endOffset': 59}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 360, 'endLine': 360, 'startOffset': 44, 'endOffset': 51}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 371, 'endLine': 371, 'startOffset': 55, 'endOffset': 62}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 415, 'endLine': 415, 'startOffset': 54, 'endOffset': 61}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 423, 'endLine': 423, 'startOffset': 51, 'endOffset': 58}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 424, 'endLine': 424, 'startOffset': 51, 'endOffset': 58}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 433, 'endLine': 433, 'startOffset': 55, 'endOffset': 62}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 434, 'endLine': 434, 'startOffset': 62, 'endOffset': 69}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 516, 'endLine': 516, 'startOffset': 44, 'endOffset': 51}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 529, 'endLine': 529, 'startOffset': 67, 'endOffset': 74}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 542, 'endLine': 542, 'startOffset': 63, 'endOffset': 70}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 548, 'endLine': 548, 'startOffset': 57, 'endOffset': 64}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 549, 'endLine': 549, 'startOffset': 64, 'endOffset': 71}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 550, 'endLine': 550, 'startOffset': 64, 'endOffset': 71}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 551, 'endLine': 551, 'startOffset': 64, 'endOffset': 71}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 552, 'endLine': 552, 'startOffset': 65, 'endOffset': 72}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 553, 'endLine': 553, 'startOffset': 65, 'endOffset': 72}, 'msg': 'Duplication.'}]}]</t>
         </is>
       </c>
       <c r="J502" t="inlineStr">
@@ -65595,7 +65643,7 @@
         </is>
       </c>
       <c r="F503" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G503" t="inlineStr">
         <is>
@@ -65604,12 +65652,12 @@
       </c>
       <c r="H503" t="inlineStr">
         <is>
-          <t>{'startLine': 101, 'endLine': 101, 'startOffset': 111, 'endOffset': 123}</t>
+          <t>{'startLine': 103, 'endLine': 103, 'startOffset': 111, 'endOffset': 123}</t>
         </is>
       </c>
       <c r="I503" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 135, 'endLine': 135, 'startOffset': 90, 'endOffset': 102}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 181, 'endLine': 181, 'startOffset': 102, 'endOffset': 114}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 206, 'endLine': 206, 'startOffset': 117, 'endOffset': 129}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 237, 'endLine': 237, 'startOffset': 107, 'endOffset': 119}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 263, 'endLine': 263, 'startOffset': 102, 'endOffset': 114}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 506, 'endLine': 506, 'startOffset': 86, 'endOffset': 98}, 'msg': 'Duplication.'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 137, 'endLine': 137, 'startOffset': 90, 'endOffset': 102}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 187, 'endLine': 187, 'startOffset': 102, 'endOffset': 114}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 212, 'endLine': 212, 'startOffset': 117, 'endOffset': 129}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 243, 'endLine': 243, 'startOffset': 107, 'endOffset': 119}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 269, 'endLine': 269, 'startOffset': 102, 'endOffset': 114}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 516, 'endLine': 516, 'startOffset': 86, 'endOffset': 98}, 'msg': 'Duplication.'}]}]</t>
         </is>
       </c>
       <c r="J503" t="inlineStr">
@@ -65722,7 +65770,7 @@
         </is>
       </c>
       <c r="F504" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="G504" t="inlineStr">
         <is>
@@ -65731,12 +65779,12 @@
       </c>
       <c r="H504" t="inlineStr">
         <is>
-          <t>{'startLine': 101, 'endLine': 101, 'startOffset': 76, 'endOffset': 87}</t>
+          <t>{'startLine': 103, 'endLine': 103, 'startOffset': 76, 'endOffset': 87}</t>
         </is>
       </c>
       <c r="I504" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 135, 'endLine': 135, 'startOffset': 63, 'endOffset': 74}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 181, 'endLine': 181, 'startOffset': 79, 'endOffset': 90}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 206, 'endLine': 206, 'startOffset': 90, 'endOffset': 101}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 237, 'endLine': 237, 'startOffset': 84, 'endOffset': 95}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 263, 'endLine': 263, 'startOffset': 71, 'endOffset': 82}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 506, 'endLine': 506, 'startOffset': 59, 'endOffset': 70}, 'msg': 'Duplication.'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 137, 'endLine': 137, 'startOffset': 63, 'endOffset': 74}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 187, 'endLine': 187, 'startOffset': 79, 'endOffset': 90}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 212, 'endLine': 212, 'startOffset': 90, 'endOffset': 101}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 243, 'endLine': 243, 'startOffset': 84, 'endOffset': 95}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 269, 'endLine': 269, 'startOffset': 71, 'endOffset': 82}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 516, 'endLine': 516, 'startOffset': 59, 'endOffset': 70}, 'msg': 'Duplication.'}]}]</t>
         </is>
       </c>
       <c r="J504" t="inlineStr">
@@ -65848,9 +65896,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F505" t="n">
-        <v>151</v>
-      </c>
+      <c r="F505" t="inlineStr"/>
       <c r="G505" t="inlineStr">
         <is>
           <t>0772e5c868dccc1f9085755bb90b4415</t>
@@ -65858,7 +65904,7 @@
       </c>
       <c r="H505" t="inlineStr">
         <is>
-          <t>{'startLine': 151, 'endLine': 151, 'startOffset': 16, 'endOffset': 18}</t>
+          <t>{'startLine': 153, 'endLine': 153, 'startOffset': 16, 'endOffset': 18}</t>
         </is>
       </c>
       <c r="I505" t="inlineStr">
@@ -65868,7 +65914,7 @@
       </c>
       <c r="J505" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K505" t="inlineStr">
@@ -65908,7 +65954,7 @@
       </c>
       <c r="R505" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T06:15:30+0000</t>
         </is>
       </c>
       <c r="S505" t="inlineStr">
@@ -65938,7 +65984,7 @@
       </c>
       <c r="X505" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y505" t="inlineStr">
@@ -65946,8 +65992,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z505" t="inlineStr"/>
-      <c r="AA505" t="inlineStr"/>
+      <c r="Z505" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA505" t="inlineStr">
+        <is>
+          <t>2025-12-28T06:15:30+0000</t>
+        </is>
+      </c>
     </row>
     <row r="506">
       <c r="A506" t="inlineStr">
@@ -65975,9 +66029,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F506" t="n">
-        <v>152</v>
-      </c>
+      <c r="F506" t="inlineStr"/>
       <c r="G506" t="inlineStr">
         <is>
           <t>5f66ee83e8de227d5f9f69bdda03bec0</t>
@@ -65985,7 +66037,7 @@
       </c>
       <c r="H506" t="inlineStr">
         <is>
-          <t>{'startLine': 152, 'endLine': 152, 'startOffset': 16, 'endOffset': 18}</t>
+          <t>{'startLine': 154, 'endLine': 154, 'startOffset': 16, 'endOffset': 18}</t>
         </is>
       </c>
       <c r="I506" t="inlineStr">
@@ -65995,7 +66047,7 @@
       </c>
       <c r="J506" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K506" t="inlineStr">
@@ -66035,7 +66087,7 @@
       </c>
       <c r="R506" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T06:15:30+0000</t>
         </is>
       </c>
       <c r="S506" t="inlineStr">
@@ -66065,7 +66117,7 @@
       </c>
       <c r="X506" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y506" t="inlineStr">
@@ -66073,8 +66125,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z506" t="inlineStr"/>
-      <c r="AA506" t="inlineStr"/>
+      <c r="Z506" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA506" t="inlineStr">
+        <is>
+          <t>2025-12-28T06:15:30+0000</t>
+        </is>
+      </c>
     </row>
     <row r="507">
       <c r="A507" t="inlineStr">
@@ -66102,9 +66162,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F507" t="n">
-        <v>288</v>
-      </c>
+      <c r="F507" t="inlineStr"/>
       <c r="G507" t="inlineStr">
         <is>
           <t>0772e5c868dccc1f9085755bb90b4415</t>
@@ -66112,7 +66170,7 @@
       </c>
       <c r="H507" t="inlineStr">
         <is>
-          <t>{'startLine': 288, 'endLine': 288, 'startOffset': 16, 'endOffset': 18}</t>
+          <t>{'startLine': 290, 'endLine': 290, 'startOffset': 16, 'endOffset': 18}</t>
         </is>
       </c>
       <c r="I507" t="inlineStr">
@@ -66122,7 +66180,7 @@
       </c>
       <c r="J507" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K507" t="inlineStr">
@@ -66162,7 +66220,7 @@
       </c>
       <c r="R507" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T06:15:30+0000</t>
         </is>
       </c>
       <c r="S507" t="inlineStr">
@@ -66192,7 +66250,7 @@
       </c>
       <c r="X507" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y507" t="inlineStr">
@@ -66200,8 +66258,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z507" t="inlineStr"/>
-      <c r="AA507" t="inlineStr"/>
+      <c r="Z507" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA507" t="inlineStr">
+        <is>
+          <t>2025-12-28T06:15:30+0000</t>
+        </is>
+      </c>
     </row>
     <row r="508">
       <c r="A508" t="inlineStr">
@@ -66229,9 +66295,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F508" t="n">
-        <v>289</v>
-      </c>
+      <c r="F508" t="inlineStr"/>
       <c r="G508" t="inlineStr">
         <is>
           <t>5f66ee83e8de227d5f9f69bdda03bec0</t>
@@ -66239,7 +66303,7 @@
       </c>
       <c r="H508" t="inlineStr">
         <is>
-          <t>{'startLine': 289, 'endLine': 289, 'startOffset': 16, 'endOffset': 18}</t>
+          <t>{'startLine': 291, 'endLine': 291, 'startOffset': 16, 'endOffset': 18}</t>
         </is>
       </c>
       <c r="I508" t="inlineStr">
@@ -66249,7 +66313,7 @@
       </c>
       <c r="J508" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K508" t="inlineStr">
@@ -66289,7 +66353,7 @@
       </c>
       <c r="R508" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T06:15:30+0000</t>
         </is>
       </c>
       <c r="S508" t="inlineStr">
@@ -66319,7 +66383,7 @@
       </c>
       <c r="X508" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y508" t="inlineStr">
@@ -66327,8 +66391,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z508" t="inlineStr"/>
-      <c r="AA508" t="inlineStr"/>
+      <c r="Z508" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA508" t="inlineStr">
+        <is>
+          <t>2025-12-28T06:15:30+0000</t>
+        </is>
+      </c>
     </row>
     <row r="509">
       <c r="A509" t="inlineStr">
@@ -66357,7 +66429,7 @@
         </is>
       </c>
       <c r="F509" t="n">
-        <v>523</v>
+        <v>533</v>
       </c>
       <c r="G509" t="inlineStr">
         <is>
@@ -66366,12 +66438,12 @@
       </c>
       <c r="H509" t="inlineStr">
         <is>
-          <t>{'startLine': 523, 'endLine': 523, 'startOffset': 55, 'endOffset': 106}</t>
+          <t>{'startLine': 533, 'endLine': 533, 'startOffset': 55, 'endOffset': 106}</t>
         </is>
       </c>
       <c r="I509" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 523, 'endLine': 523, 'startOffset': 48, 'endOffset': 49}, 'msg': 'Parent ternary operator'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 533, 'endLine': 533, 'startOffset': 48, 'endOffset': 49}, 'msg': 'Parent ternary operator'}]}]</t>
         </is>
       </c>
       <c r="J509" t="inlineStr">
@@ -66484,7 +66556,7 @@
         </is>
       </c>
       <c r="F510" t="n">
-        <v>538</v>
+        <v>548</v>
       </c>
       <c r="G510" t="inlineStr">
         <is>
@@ -66493,12 +66565,12 @@
       </c>
       <c r="H510" t="inlineStr">
         <is>
-          <t>{'startLine': 538, 'endLine': 538, 'startOffset': 86, 'endOffset': 119}</t>
+          <t>{'startLine': 548, 'endLine': 548, 'startOffset': 86, 'endOffset': 119}</t>
         </is>
       </c>
       <c r="I510" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 540, 'endLine': 540, 'startOffset': 93, 'endOffset': 126}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 542, 'endLine': 542, 'startOffset': 94, 'endOffset': 127}, 'msg': 'Duplication.'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 550, 'endLine': 550, 'startOffset': 93, 'endOffset': 126}, 'msg': 'Duplication.'}]}, {'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/chart/render.php', 'textRange': {'startLine': 552, 'endLine': 552, 'startOffset': 94, 'endOffset': 127}, 'msg': 'Duplication.'}]}]</t>
         </is>
       </c>
       <c r="J510" t="inlineStr">
@@ -67372,9 +67444,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F517" t="n">
-        <v>12</v>
-      </c>
+      <c r="F517" t="inlineStr"/>
       <c r="G517" t="inlineStr">
         <is>
           <t>0f73e63a91f97d12d77517b8f5dc749f</t>
@@ -67392,7 +67462,7 @@
       </c>
       <c r="J517" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K517" t="inlineStr">
@@ -67432,7 +67502,7 @@
       </c>
       <c r="R517" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T06:15:30+0000</t>
         </is>
       </c>
       <c r="S517" t="inlineStr">
@@ -67462,7 +67532,7 @@
       </c>
       <c r="X517" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y517" t="inlineStr">
@@ -67470,8 +67540,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z517" t="inlineStr"/>
-      <c r="AA517" t="inlineStr"/>
+      <c r="Z517" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA517" t="inlineStr">
+        <is>
+          <t>2025-12-28T06:15:30+0000</t>
+        </is>
+      </c>
     </row>
     <row r="518">
       <c r="A518" t="inlineStr">
@@ -67499,9 +67577,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F518" t="n">
-        <v>16</v>
-      </c>
+      <c r="F518" t="inlineStr"/>
       <c r="G518" t="inlineStr">
         <is>
           <t>28cdf959450ab28df4eed6fa207d7214</t>
@@ -67519,7 +67595,7 @@
       </c>
       <c r="J518" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K518" t="inlineStr">
@@ -67559,7 +67635,7 @@
       </c>
       <c r="R518" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T06:15:30+0000</t>
         </is>
       </c>
       <c r="S518" t="inlineStr">
@@ -67589,7 +67665,7 @@
       </c>
       <c r="X518" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y518" t="inlineStr">
@@ -67597,8 +67673,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z518" t="inlineStr"/>
-      <c r="AA518" t="inlineStr"/>
+      <c r="Z518" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA518" t="inlineStr">
+        <is>
+          <t>2025-12-28T06:15:30+0000</t>
+        </is>
+      </c>
     </row>
     <row r="519">
       <c r="A519" t="inlineStr">
@@ -67626,9 +67710,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F519" t="n">
-        <v>17</v>
-      </c>
+      <c r="F519" t="inlineStr"/>
       <c r="G519" t="inlineStr">
         <is>
           <t>84bb3dd0f91605e62be53bff2dac3807</t>
@@ -67646,7 +67728,7 @@
       </c>
       <c r="J519" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K519" t="inlineStr">
@@ -67686,7 +67768,7 @@
       </c>
       <c r="R519" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T06:15:30+0000</t>
         </is>
       </c>
       <c r="S519" t="inlineStr">
@@ -67716,7 +67798,7 @@
       </c>
       <c r="X519" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y519" t="inlineStr">
@@ -67724,8 +67806,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z519" t="inlineStr"/>
-      <c r="AA519" t="inlineStr"/>
+      <c r="Z519" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA519" t="inlineStr">
+        <is>
+          <t>2025-12-28T06:15:30+0000</t>
+        </is>
+      </c>
     </row>
     <row r="520">
       <c r="A520" t="inlineStr">
@@ -67754,7 +67844,7 @@
         </is>
       </c>
       <c r="F520" t="n">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="G520" t="inlineStr">
         <is>
@@ -67763,12 +67853,12 @@
       </c>
       <c r="H520" t="inlineStr">
         <is>
-          <t>{'startLine': 19, 'endLine': 19, 'startOffset': 40, 'endOffset': 71}</t>
+          <t>{'startLine': 24, 'endLine': 24, 'startOffset': 40, 'endOffset': 71}</t>
         </is>
       </c>
       <c r="I520" t="inlineStr">
         <is>
-          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/confidence-meter/render.php', 'textRange': {'startLine': 19, 'endLine': 19, 'startOffset': 28, 'endOffset': 29}, 'msg': 'Parent ternary operator'}]}]</t>
+          <t>[{'locations': [{'component': '100PercentTuna_dancing-octopi:kunaal-theme/blocks/confidence-meter/render.php', 'textRange': {'startLine': 24, 'endLine': 24, 'startOffset': 28, 'endOffset': 29}, 'msg': 'Parent ternary operator'}]}]</t>
         </is>
       </c>
       <c r="J520" t="inlineStr">
@@ -73522,9 +73612,7 @@
           <t>100PercentTuna_dancing-octopi</t>
         </is>
       </c>
-      <c r="F565" t="n">
-        <v>215</v>
-      </c>
+      <c r="F565" t="inlineStr"/>
       <c r="G565" t="inlineStr">
         <is>
           <t>32faa51932da20adb11d32620be0712b</t>
@@ -73542,7 +73630,7 @@
       </c>
       <c r="J565" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>CLOSED</t>
         </is>
       </c>
       <c r="K565" t="inlineStr">
@@ -73582,7 +73670,7 @@
       </c>
       <c r="R565" t="inlineStr">
         <is>
-          <t>2025-12-27T20:17:45+0000</t>
+          <t>2025-12-28T06:15:30+0000</t>
         </is>
       </c>
       <c r="S565" t="inlineStr">
@@ -73612,7 +73700,7 @@
       </c>
       <c r="X565" t="inlineStr">
         <is>
-          <t>OPEN</t>
+          <t>FIXED</t>
         </is>
       </c>
       <c r="Y565" t="inlineStr">
@@ -73620,8 +73708,16 @@
           <t>dancing-octopi</t>
         </is>
       </c>
-      <c r="Z565" t="inlineStr"/>
-      <c r="AA565" t="inlineStr"/>
+      <c r="Z565" t="inlineStr">
+        <is>
+          <t>FIXED</t>
+        </is>
+      </c>
+      <c r="AA565" t="inlineStr">
+        <is>
+          <t>2025-12-28T06:15:30+0000</t>
+        </is>
+      </c>
     </row>
     <row r="566">
       <c r="A566" t="inlineStr">
@@ -74176,7 +74272,7 @@
         </is>
       </c>
       <c r="F570" t="n">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="G570" t="inlineStr">
         <is>
@@ -74185,7 +74281,7 @@
       </c>
       <c r="H570" t="inlineStr">
         <is>
-          <t>{'startLine': 278, 'endLine': 278, 'startOffset': 9, 'endOffset': 31}</t>
+          <t>{'startLine': 283, 'endLine': 283, 'startOffset': 9, 'endOffset': 31}</t>
         </is>
       </c>
       <c r="I570" t="inlineStr">

</xml_diff>